<commit_message>
Updated a few README.md & Removed the scripts/models/ directory.
It was useless.
</commit_message>
<xml_diff>
--- a/user/example/données_servo.xlsx
+++ b/user/example/données_servo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nono_\SynologyDrive\GitHub\smov\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nono_\SynologyDrive\GitHub\smov\user\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E1561D-1B51-4AFB-8EF2-4FE3F0BEE384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D458FE33-F331-49A9-B162-516A20444916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{202B0410-E24E-4D9C-955B-905AFDAB2AE3}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{202B0410-E24E-4D9C-955B-905AFDAB2AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Nom</t>
   </si>
@@ -81,6 +70,33 @@
   </si>
   <si>
     <t>Ecart Min</t>
+  </si>
+  <si>
+    <t>AVMG</t>
+  </si>
+  <si>
+    <t>ARMG</t>
+  </si>
+  <si>
+    <t>AVMD</t>
+  </si>
+  <si>
+    <t>Min: Le plus haut</t>
+  </si>
+  <si>
+    <t>Max: Le plus bas</t>
+  </si>
+  <si>
+    <t>555 (angle non parfait)</t>
+  </si>
+  <si>
+    <t>ARMD</t>
+  </si>
+  <si>
+    <t>REPLACER LE SERVO (75)</t>
+  </si>
+  <si>
+    <t>AVJG</t>
   </si>
 </sst>
 </file>
@@ -432,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB0C8FC-AE37-4EC1-BA88-65E1AE8F61DF}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +502,7 @@
         <v>90</v>
       </c>
       <c r="H2">
-        <v>135</v>
+        <v>-135</v>
       </c>
       <c r="I2">
         <v>15</v>
@@ -512,7 +528,7 @@
         <v>135</v>
       </c>
       <c r="I3">
-        <v>15</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -535,7 +551,7 @@
         <v>100</v>
       </c>
       <c r="I4">
-        <v>15</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -555,10 +571,108 @@
         <v>110</v>
       </c>
       <c r="H5">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="I5">
         <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>220</v>
+      </c>
+      <c r="F6">
+        <v>90</v>
+      </c>
+      <c r="G6">
+        <v>400</v>
+      </c>
+      <c r="H6">
+        <v>180</v>
+      </c>
+      <c r="I6">
+        <v>-130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>460</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>290</v>
+      </c>
+      <c r="H7">
+        <v>-170</v>
+      </c>
+      <c r="I7">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>340</v>
+      </c>
+      <c r="F8">
+        <v>200</v>
+      </c>
+      <c r="G8">
+        <v>505</v>
+      </c>
+      <c r="H8">
+        <v>165</v>
+      </c>
+      <c r="I8">
+        <v>-140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed (the first part) of the parameters system inside the States package.
Also fixed a few other issues inside that package.
</commit_message>
<xml_diff>
--- a/user/example/données_servo.xlsx
+++ b/user/example/données_servo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nono_\SynologyDrive\GitHub\smov\user\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D458FE33-F331-49A9-B162-516A20444916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DB6260-84F5-4BD1-B233-7E4FD69ECA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{202B0410-E24E-4D9C-955B-905AFDAB2AE3}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{202B0410-E24E-4D9C-955B-905AFDAB2AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Nom</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>AVJG</t>
+  </si>
+  <si>
+    <t>Valeur Absolue</t>
+  </si>
+  <si>
+    <t>Angle</t>
   </si>
 </sst>
 </file>
@@ -448,15 +454,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB0C8FC-AE37-4EC1-BA88-65E1AE8F61DF}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,7 +491,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -508,7 +514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -531,7 +537,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -554,7 +560,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -577,7 +583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -600,7 +606,7 @@
         <v>-130</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -623,7 +629,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -646,7 +652,7 @@
         <v>-140</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -657,7 +663,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -665,14 +671,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>445</v>
+      </c>
+      <c r="B17">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>230</v>
+      </c>
+      <c r="B18">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>338</v>
+      </c>
+      <c r="B19">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>115</v>
+      </c>
+      <c r="B20">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>